<commit_message>
Add Excel and PowerPoint
</commit_message>
<xml_diff>
--- a/Planejamento_01.xlsx
+++ b/Planejamento_01.xlsx
@@ -876,20 +876,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1449,7 +1440,7 @@
   <dimension ref="A1:S48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L39" sqref="L39:Q39"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1464,1044 +1455,1044 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" ht="15.75" spans="1:19">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="4" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3">
         <v>1</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="K3" s="6" t="s">
+      <c r="I3" s="7"/>
+      <c r="K3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3">
         <v>1</v>
       </c>
-      <c r="S3" s="10"/>
+      <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="10"/>
-      <c r="K4" s="11" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="7"/>
+      <c r="K4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="10"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="10"/>
-      <c r="K5" s="7" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="7"/>
+      <c r="K5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="10"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="7"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="10"/>
-      <c r="K6" s="6" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="7"/>
+      <c r="K6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="10"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="10"/>
-      <c r="K7" s="6" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="7"/>
+      <c r="K7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="10"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="10"/>
-      <c r="K8" s="6" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="7"/>
+      <c r="K8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="10"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="7"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="10"/>
-      <c r="K9" s="6" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="7"/>
+      <c r="K9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="10"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="10"/>
-      <c r="K10" s="6" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="7"/>
+      <c r="K10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="10"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="7"/>
     </row>
     <row r="11" spans="2:19">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="K11" s="6" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="K11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-      <c r="S11" s="10"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="7"/>
     </row>
     <row r="12" spans="2:19">
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="K12" s="6" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="K12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="10"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="7"/>
     </row>
     <row r="13" spans="2:19">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="K13" s="6" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="K13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="10"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="7"/>
     </row>
     <row r="14" spans="2:19">
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="K14" s="6" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="K14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="10"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="7"/>
     </row>
     <row r="15" spans="2:19">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="K15" s="6" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="K15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="10"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="7"/>
     </row>
     <row r="16" spans="2:19">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="K16" s="6" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="K16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="6"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="10"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="7"/>
     </row>
     <row r="17" spans="2:19">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="K17" s="6" t="s">
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="K17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
-      <c r="S17" s="10"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="7"/>
     </row>
     <row r="18" ht="21" spans="1:19">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="K18" s="6" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="K18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="6"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="10"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="7"/>
     </row>
     <row r="19" ht="15.75" spans="1:19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="K19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="10"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="7"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3">
         <v>1</v>
       </c>
-      <c r="I20" s="10"/>
-      <c r="K20" s="6" t="s">
+      <c r="I20" s="7"/>
+      <c r="K20" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
-      <c r="P20" s="6"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="10"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="7"/>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="9" t="s">
+      <c r="A21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="10"/>
-      <c r="K21" s="6" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="7"/>
+      <c r="K21" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="6"/>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="10"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="7"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="10"/>
-      <c r="K22" s="6" t="s">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="7"/>
+      <c r="K22" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="L22" s="6"/>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="10"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="7"/>
     </row>
     <row r="23" spans="1:19">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="10"/>
-      <c r="K23" s="6" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="7"/>
+      <c r="K23" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="6"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
-      <c r="S23" s="10"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="7"/>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="10"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="10"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="10"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="7"/>
     </row>
     <row r="28" spans="2:8">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:8">
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" ht="21" spans="2:19">
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
       <c r="K30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2"/>
-      <c r="R30" s="2"/>
-      <c r="S30" s="2"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
     </row>
     <row r="31" ht="15.75" spans="2:19">
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="K31" s="3" t="s">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="K31" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="5"/>
-      <c r="R31" s="4" t="s">
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="S31" s="4" t="s">
+      <c r="S31" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="32" spans="2:19">
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="K32" s="6" t="s">
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="K32" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6">
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3">
         <v>1</v>
       </c>
-      <c r="S32" s="10"/>
+      <c r="S32" s="7"/>
     </row>
     <row r="33" ht="21" spans="1:19">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="K33" s="9" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="K33" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L33" s="6"/>
-      <c r="M33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
-      <c r="S33" s="10"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="7"/>
     </row>
     <row r="34" ht="15.75" spans="1:19">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="4" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="I34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="K34" s="7" t="s">
+      <c r="K34" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
-      <c r="O34" s="6"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="10"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="7"/>
     </row>
     <row r="35" spans="1:19">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3">
         <v>1</v>
       </c>
-      <c r="I35" s="10"/>
-      <c r="K35" s="6" t="s">
+      <c r="I35" s="7"/>
+      <c r="K35" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="L35" s="6"/>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6"/>
-      <c r="O35" s="6"/>
-      <c r="P35" s="6"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
-      <c r="S35" s="10"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="7"/>
     </row>
     <row r="36" spans="1:19">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="10"/>
-      <c r="K36" s="6" t="s">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="7"/>
+      <c r="K36" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L36" s="6"/>
-      <c r="M36" s="6"/>
-      <c r="N36" s="6"/>
-      <c r="O36" s="6"/>
-      <c r="P36" s="6"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
-      <c r="S36" s="10"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="7"/>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="10"/>
-      <c r="K37" s="6" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="7"/>
+      <c r="K37" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
-      <c r="N37" s="6"/>
-      <c r="O37" s="6"/>
-      <c r="P37" s="6"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
-      <c r="S37" s="10"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="7"/>
     </row>
     <row r="38" spans="1:19">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="10"/>
-      <c r="K38" s="6" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="7"/>
+      <c r="K38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="6"/>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="10"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="7"/>
     </row>
     <row r="39" spans="1:19">
-      <c r="A39" s="6" t="s">
+      <c r="A39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="10"/>
-      <c r="K39" s="6" t="s">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="7"/>
+      <c r="K39" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="L39" s="6"/>
-      <c r="M39" s="6"/>
-      <c r="N39" s="6"/>
-      <c r="O39" s="6"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
-      <c r="S39" s="10"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="7"/>
     </row>
     <row r="40" spans="1:19">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="10"/>
-      <c r="K40" s="6" t="s">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="7"/>
+      <c r="K40" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6"/>
-      <c r="O40" s="6"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="10"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="7"/>
     </row>
     <row r="41" spans="1:19">
-      <c r="A41" s="6" t="s">
+      <c r="A41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="10"/>
-      <c r="K41" s="6" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="7"/>
+      <c r="K41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L41" s="6"/>
-      <c r="M41" s="6"/>
-      <c r="N41" s="6"/>
-      <c r="O41" s="6"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="10"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="7"/>
     </row>
     <row r="42" spans="1:19">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="10"/>
-      <c r="K42" s="6" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="7"/>
+      <c r="K42" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L42" s="6"/>
-      <c r="M42" s="6"/>
-      <c r="N42" s="6"/>
-      <c r="O42" s="6"/>
-      <c r="P42" s="6"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
-      <c r="S42" s="10"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="7"/>
     </row>
     <row r="43" customFormat="1" spans="1:19">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="10"/>
-      <c r="K43" s="6" t="s">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="7"/>
+      <c r="K43" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="10"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="7"/>
     </row>
     <row r="44" customFormat="1" spans="1:19">
-      <c r="A44" s="6" t="s">
+      <c r="A44" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="10"/>
-      <c r="K44" s="6" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="7"/>
+      <c r="K44" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="L44" s="6"/>
-      <c r="M44" s="6"/>
-      <c r="N44" s="6"/>
-      <c r="O44" s="6"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="10"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="7"/>
     </row>
     <row r="45" customFormat="1" spans="1:19">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="10"/>
-      <c r="K45" s="6" t="s">
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="7"/>
+      <c r="K45" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
-      <c r="N45" s="6"/>
-      <c r="O45" s="6"/>
-      <c r="P45" s="6"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
-      <c r="S45" s="10"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="7"/>
     </row>
     <row r="46" customFormat="1" spans="1:9">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="10"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="7"/>
     </row>
     <row r="47" customFormat="1" spans="1:9">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="10"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="7"/>
     </row>
     <row r="48" customFormat="1" spans="1:9">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="10"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="87">

</xml_diff>